<commit_message>
Updates to crossing stress
</commit_message>
<xml_diff>
--- a/pybna/sql/stress/tables/stress_crossing.xlsx
+++ b/pybna/sql/stress/tables/stress_crossing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pybna\pybna\sql\stress\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{684B4C67-E277-4B35-9372-9D4EB7D3D85F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A818F6-DDD9-4600-8B74-AFB431AEC254}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8882EFA-E71A-44FB-864D-416D76E01D0F}"/>
+    <workbookView xWindow="17730" yWindow="3270" windowWidth="21600" windowHeight="11775" xr2:uid="{B8882EFA-E71A-44FB-864D-416D76E01D0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="11">
   <si>
     <t>control</t>
   </si>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB73C8A-95F0-43C4-86E2-5746CF75369C}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +465,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,13 +484,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -515,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -529,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,13 +543,13 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -557,13 +557,13 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,13 +571,13 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,27 +585,27 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>99</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -627,47 +627,41 @@
         <v>99</v>
       </c>
       <c r="C15">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>99</v>
+      </c>
+      <c r="C16">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
       <c r="B17">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C17">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -692,10 +686,10 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -709,16 +703,16 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -746,13 +740,13 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -763,13 +757,13 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,13 +774,13 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,13 +791,13 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,13 +808,13 @@
         <v>5</v>
       </c>
       <c r="C26">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,10 +822,10 @@
         <v>7</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -845,16 +839,16 @@
         <v>7</v>
       </c>
       <c r="B28">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -862,66 +856,134 @@
         <v>7</v>
       </c>
       <c r="B29">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30">
         <v>99</v>
       </c>
       <c r="C30">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31">
         <v>99</v>
       </c>
       <c r="C31">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>99</v>
+      </c>
+      <c r="C32">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>99</v>
+      </c>
+      <c r="C33">
+        <v>99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>99</v>
+      </c>
+      <c r="C34">
+        <v>99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>99</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B32">
-        <v>99</v>
-      </c>
-      <c r="C32">
-        <v>99</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32">
+      <c r="B36">
+        <v>99</v>
+      </c>
+      <c r="C36">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36">
         <v>1</v>
       </c>
     </row>

</xml_diff>